<commit_message>
22/08/2023 Just 35 min content remaining to complete Nodejs and Express js
</commit_message>
<xml_diff>
--- a/Data-Science/Projects/Live-Project/Sub-Cateogrised=Expenses-ALL.xlsx
+++ b/Data-Science/Projects/Live-Project/Sub-Cateogrised=Expenses-ALL.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1945,14 +1945,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1982,9 +1989,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2289,10 +2299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B636"/>
+  <dimension ref="A1:B638"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A535" workbookViewId="0">
+      <selection activeCell="G549" sqref="G549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6661,7 +6671,7 @@
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A546" s="1" t="s">
+      <c r="A546" s="2" t="s">
         <v>545</v>
       </c>
       <c r="B546">
@@ -7386,6 +7396,12 @@
       </c>
       <c r="B636">
         <v>7800</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B638">
+        <f>SUM(B1:B636)</f>
+        <v>3248975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>